<commit_message>
annotate script, reorder chunks
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -41,31 +41,31 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">age</t>
+    <t xml:space="preserve">Age at Diagnosis</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">reported_gender</t>
+    <t xml:space="preserve">Reported Gender</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">race</t>
+    <t xml:space="preserve">Reported Race</t>
   </si>
   <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">ethnicity</t>
+    <t xml:space="preserve">Reported Ethnicity</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">mol_sub_group</t>
+    <t xml:space="preserve">Molecular Subgroup</t>
   </si>
   <si>
     <t xml:space="preserve">6</t>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">7</t>
   </si>
   <si>
-    <t xml:space="preserve">extent_of_tumor_resection</t>
+    <t xml:space="preserve">Extent of Tumor Resection</t>
   </si>
   <si>
     <t xml:space="preserve">8</t>
@@ -446,7 +446,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.217969285650778</v>
+        <v>0.217969285650775</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.610738926107389</v>
+        <v>0.606339366063394</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +490,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0342965703429657</v>
+        <v>0.0331966803319668</v>
       </c>
     </row>
     <row r="7">
@@ -501,7 +501,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.219278072192781</v>
+        <v>0.228377162283772</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.77992200779922</v>
+        <v>0.787121287871213</v>
       </c>
     </row>
     <row r="9">
@@ -523,7 +523,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0607939206079392</v>
+        <v>0.0612938706129387</v>
       </c>
     </row>
     <row r="10">
@@ -534,7 +534,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>0.043876295317301</v>
+        <v>0.0438762953173008</v>
       </c>
     </row>
     <row r="11">
@@ -581,7 +581,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.278583212588569</v>
+        <v>0.278583212588568</v>
       </c>
     </row>
     <row r="3">
@@ -592,7 +592,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.388361163883612</v>
+        <v>0.405059494050595</v>
       </c>
     </row>
     <row r="4">
@@ -625,7 +625,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.259274072592741</v>
+        <v>0.262573742625737</v>
       </c>
     </row>
     <row r="7">
@@ -636,7 +636,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.27957204279572</v>
+        <v>0.278672132786721</v>
       </c>
     </row>
     <row r="8">
@@ -647,7 +647,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.966003399660034</v>
+        <v>0.966403359664034</v>
       </c>
     </row>
     <row r="9">
@@ -680,7 +680,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>0.743616658580256</v>
+        <v>0.743616658580255</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +727,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.501549845015498</v>
+        <v>0.505149485051495</v>
       </c>
     </row>
     <row r="4">
@@ -760,7 +760,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.013998600139986</v>
+        <v>0.0158984101589841</v>
       </c>
     </row>
     <row r="7">
@@ -771,7 +771,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.615938406159384</v>
+        <v>0.618238176182382</v>
       </c>
     </row>
     <row r="8">
@@ -793,7 +793,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>0.124845238053224</v>
+        <v>0.124845238053223</v>
       </c>
     </row>
     <row r="10">
@@ -804,7 +804,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="n">
-        <v>0.259262165005024</v>
+        <v>0.259262165005025</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +851,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.355464453554645</v>
+        <v>0.368663133686631</v>
       </c>
     </row>
     <row r="4">
@@ -873,7 +873,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0000999900009999</v>
+        <v>0.0007999200079992</v>
       </c>
     </row>
     <row r="6">
@@ -884,7 +884,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.497650234976502</v>
+        <v>0.498550144985501</v>
       </c>
     </row>
     <row r="7">
@@ -895,7 +895,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.268873112688731</v>
+        <v>0.284671532846715</v>
       </c>
     </row>
     <row r="8">
@@ -906,7 +906,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.176182381761824</v>
+        <v>0.171182881711829</v>
       </c>
     </row>
     <row r="9">
@@ -917,7 +917,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.215578442155784</v>
+        <v>0.212678732126787</v>
       </c>
     </row>
     <row r="10">
@@ -939,7 +939,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>0.541788422608162</v>
+        <v>0.541788422608163</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.797420257974203</v>
+        <v>0.7996200379962</v>
       </c>
     </row>
     <row r="4">
@@ -1019,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.839216078392161</v>
+        <v>0.837116288371163</v>
       </c>
     </row>
     <row r="7">
@@ -1030,7 +1030,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0193980601939806</v>
+        <v>0.0172982701729827</v>
       </c>
     </row>
     <row r="8">
@@ -1041,7 +1041,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.67043295670433</v>
+        <v>0.668633136686331</v>
       </c>
     </row>
     <row r="9">
@@ -1052,7 +1052,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.972802719728027</v>
+        <v>0.975602439756024</v>
       </c>
     </row>
     <row r="10">
@@ -1063,7 +1063,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>0.415013092936938</v>
+        <v>0.415013092936939</v>
       </c>
     </row>
     <row r="11">
@@ -1110,7 +1110,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0928659156743259</v>
+        <v>0.0928659156743261</v>
       </c>
     </row>
     <row r="3">
@@ -1121,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.941105889411059</v>
+        <v>0.942105789421058</v>
       </c>
     </row>
     <row r="4">
@@ -1143,7 +1143,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0004999500049995</v>
+        <v>0.0003999600039996</v>
       </c>
     </row>
     <row r="6">
@@ -1154,7 +1154,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.684831516848315</v>
+        <v>0.68953104689531</v>
       </c>
     </row>
     <row r="7">
@@ -1165,7 +1165,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.31016898310169</v>
+        <v>0.311968803119688</v>
       </c>
     </row>
     <row r="8">
@@ -1176,7 +1176,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="n">
-        <v>0.203179682031797</v>
+        <v>0.201379862013799</v>
       </c>
     </row>
     <row r="9">
@@ -1256,7 +1256,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0004999500049995</v>
+        <v>0.0002999700029997</v>
       </c>
     </row>
     <row r="5">
@@ -1267,7 +1267,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.156884311568843</v>
+        <v>0.149185081491851</v>
       </c>
     </row>
     <row r="6">
@@ -1278,7 +1278,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0588941105889411</v>
+        <v>0.0546945305469453</v>
       </c>
     </row>
     <row r="7">
@@ -1289,7 +1289,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.301469853014699</v>
+        <v>0.294770522947705</v>
       </c>
     </row>
     <row r="8">
@@ -1300,7 +1300,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3999600039996</v>
+        <v>0.398860113988601</v>
       </c>
     </row>
     <row r="9">
@@ -1358,7 +1358,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0575209855960224</v>
+        <v>0.0575209855960223</v>
       </c>
     </row>
     <row r="3">
@@ -1369,7 +1369,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.304769523047695</v>
+        <v>0.300569943005699</v>
       </c>
     </row>
     <row r="4">
@@ -1391,7 +1391,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.284871512848715</v>
+        <v>0.291870812918708</v>
       </c>
     </row>
     <row r="6">
@@ -1413,7 +1413,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.221777822217778</v>
+        <v>0.221877812218778</v>
       </c>
     </row>
     <row r="8">
@@ -1482,7 +1482,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.563235079302387</v>
+        <v>0.563235079302386</v>
       </c>
     </row>
     <row r="3">
@@ -1493,7 +1493,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.916308369163084</v>
+        <v>0.905509449055094</v>
       </c>
     </row>
     <row r="4">
@@ -1515,7 +1515,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0000999900009999</v>
+        <v>0.0001999800019998</v>
       </c>
     </row>
     <row r="6">
@@ -1526,7 +1526,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.247375262473753</v>
+        <v>0.250874912508749</v>
       </c>
     </row>
     <row r="7">
@@ -1537,7 +1537,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.849315068493151</v>
+        <v>0.854214578542146</v>
       </c>
     </row>
     <row r="8">
@@ -1617,7 +1617,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.201279872012799</v>
+        <v>0.201379862013799</v>
       </c>
     </row>
     <row r="4">
@@ -1650,7 +1650,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.51964803519648</v>
+        <v>0.521047895210479</v>
       </c>
     </row>
     <row r="7">
@@ -1661,7 +1661,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.79042095790421</v>
+        <v>0.784521547845215</v>
       </c>
     </row>
     <row r="8">
@@ -1672,7 +1672,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.697030296970303</v>
+        <v>0.710928907109289</v>
       </c>
     </row>
     <row r="9">
@@ -1683,7 +1683,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.263573642635736</v>
+        <v>0.261273872612739</v>
       </c>
     </row>
     <row r="10">
@@ -1741,7 +1741,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.89064328429506</v>
+        <v>0.890643284295059</v>
       </c>
     </row>
     <row r="3">
@@ -1752,7 +1752,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.776522347765223</v>
+        <v>0.783321667833217</v>
       </c>
     </row>
     <row r="4">
@@ -1785,7 +1785,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.467053294670533</v>
+        <v>0.477352264773523</v>
       </c>
     </row>
     <row r="7">
@@ -1796,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.292470752924708</v>
+        <v>0.297670232976702</v>
       </c>
     </row>
     <row r="8">
@@ -1807,7 +1807,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.835416458354165</v>
+        <v>0.836516348365164</v>
       </c>
     </row>
     <row r="9">
@@ -1887,7 +1887,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.915908409159084</v>
+        <v>0.913008699130087</v>
       </c>
     </row>
     <row r="4">
@@ -1909,7 +1909,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.528547145285471</v>
+        <v>0.520847915208479</v>
       </c>
     </row>
     <row r="6">
@@ -1920,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.926707329267073</v>
+        <v>0.925207479252075</v>
       </c>
     </row>
     <row r="7">
@@ -1931,7 +1931,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.715028497150285</v>
+        <v>0.724727527247275</v>
       </c>
     </row>
     <row r="8">
@@ -1942,7 +1942,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="n">
-        <v>0.947205279472053</v>
+        <v>0.944905509449055</v>
       </c>
     </row>
     <row r="9">
@@ -1964,7 +1964,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0419697378487614</v>
+        <v>0.0419697378487613</v>
       </c>
     </row>
   </sheetData>
@@ -2011,7 +2011,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.122187781221878</v>
+        <v>0.126887311268873</v>
       </c>
     </row>
     <row r="4">
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.847715228477152</v>
+        <v>0.841915808419158</v>
       </c>
     </row>
     <row r="7">
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.484051594840516</v>
+        <v>0.484551544845515</v>
       </c>
     </row>
     <row r="8">
@@ -2066,7 +2066,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="n">
-        <v>0.163283671632837</v>
+        <v>0.166383361663834</v>
       </c>
     </row>
     <row r="9">
@@ -2088,7 +2088,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="n">
-        <v>0.588256408874303</v>
+        <v>0.588256408874304</v>
       </c>
     </row>
   </sheetData>
@@ -2135,7 +2135,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.615938406159384</v>
+        <v>0.628537146285371</v>
       </c>
     </row>
     <row r="4">
@@ -2157,7 +2157,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0084991500849915</v>
+        <v>0.0076992300769923</v>
       </c>
     </row>
     <row r="6">
@@ -2168,7 +2168,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.361163883611639</v>
+        <v>0.369163083691631</v>
       </c>
     </row>
     <row r="7">
@@ -2179,7 +2179,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.282871712828717</v>
+        <v>0.277872212778722</v>
       </c>
     </row>
     <row r="8">
@@ -2201,7 +2201,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>0.344188269692039</v>
+        <v>0.344188269692038</v>
       </c>
     </row>
     <row r="10">
@@ -2259,7 +2259,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.738326167383262</v>
+        <v>0.733826617338266</v>
       </c>
     </row>
     <row r="4">
@@ -2281,7 +2281,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0045995400459954</v>
+        <v>0.0038996100389961</v>
       </c>
     </row>
     <row r="6">
@@ -2292,7 +2292,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.173482651734827</v>
+        <v>0.165083491650835</v>
       </c>
     </row>
     <row r="7">
@@ -2303,7 +2303,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.57954204579542</v>
+        <v>0.58004199580042</v>
       </c>
     </row>
     <row r="8">
@@ -2372,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.744389813120938</v>
+        <v>0.744389813120937</v>
       </c>
     </row>
     <row r="3">
@@ -2383,7 +2383,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0968903109689031</v>
+        <v>0.0970902909709029</v>
       </c>
     </row>
     <row r="4">
@@ -2405,7 +2405,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0005999400059994</v>
       </c>
     </row>
     <row r="6">
@@ -2416,7 +2416,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.715228477152285</v>
+        <v>0.71002899710029</v>
       </c>
     </row>
     <row r="7">
@@ -2449,7 +2449,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>0.715220319009892</v>
+        <v>0.715220319009891</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
rm cancer predisposition, update with BRAF V600E subtype
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -1,109 +1,110 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chop365-my.sharepoint.com/personal/corbettr_chop_edu/Documents/Desktop/pbta-ancestry/analyses/demo-clin-stats/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_47D54D52D6C7FCCF425439838D0FC8DAC6643FBD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09F47B64-EEF0-224A-838E-E198FA29C3F8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-29880" yWindow="2760" windowWidth="19120" windowHeight="13120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Low-grade glioma" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Non-neoplastic tumor" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Mixed neuronal-glial tumor" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Medulloblastoma" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Schwannoma" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Mesenchymal tumor" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Germ cell tumor" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Craniopharyngioma" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Other tumor" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Ependymoma" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="DIPG or DMG" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="ATRT" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Other high-grade glioma" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Meningioma" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Neurofibroma plexiform" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Oligodendroglioma" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Low-grade glioma" sheetId="1" r:id="rId1"/>
+    <sheet name="Non-neoplastic tumor" sheetId="2" r:id="rId2"/>
+    <sheet name="Mixed neuronal-glial tumor" sheetId="3" r:id="rId3"/>
+    <sheet name="Medulloblastoma" sheetId="4" r:id="rId4"/>
+    <sheet name="Schwannoma" sheetId="5" r:id="rId5"/>
+    <sheet name="Mesenchymal tumor" sheetId="6" r:id="rId6"/>
+    <sheet name="Germ cell tumor" sheetId="7" r:id="rId7"/>
+    <sheet name="Craniopharyngioma" sheetId="8" r:id="rId8"/>
+    <sheet name="Other tumor" sheetId="9" r:id="rId9"/>
+    <sheet name="Ependymoma" sheetId="10" r:id="rId10"/>
+    <sheet name="DIPG or DMG" sheetId="11" r:id="rId11"/>
+    <sheet name="ATRT" sheetId="12" r:id="rId12"/>
+    <sheet name="Other high-grade glioma" sheetId="13" r:id="rId13"/>
+    <sheet name="Meningioma" sheetId="14" r:id="rId14"/>
+    <sheet name="Neurofibroma plexiform" sheetId="15" r:id="rId15"/>
+    <sheet name="Oligodendroglioma" sheetId="16" r:id="rId16"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="21">
   <si>
-    <t xml:space="preserve"/>
+    <t/>
   </si>
   <si>
-    <t xml:space="preserve">term</t>
+    <t>term</t>
   </si>
   <si>
-    <t xml:space="preserve">pvalue</t>
+    <t>pvalue</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
+    <t>1</t>
   </si>
   <si>
-    <t xml:space="preserve">Age at Diagnosis</t>
+    <t>Age at Diagnosis</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t>2</t>
   </si>
   <si>
-    <t xml:space="preserve">Reported Gender</t>
+    <t>Reported Gender</t>
   </si>
   <si>
-    <t xml:space="preserve">3</t>
+    <t>3</t>
   </si>
   <si>
-    <t xml:space="preserve">Reported Race</t>
+    <t>Reported Race</t>
   </si>
   <si>
-    <t xml:space="preserve">4</t>
+    <t>4</t>
   </si>
   <si>
-    <t xml:space="preserve">Reported Ethnicity</t>
+    <t>Reported Ethnicity</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
+    <t>5</t>
   </si>
   <si>
-    <t xml:space="preserve">Molecular Subgroup</t>
+    <t>Molecular Subgroup</t>
   </si>
   <si>
-    <t xml:space="preserve">6</t>
+    <t>6</t>
   </si>
   <si>
-    <t xml:space="preserve">CNS region</t>
+    <t>CNS region</t>
   </si>
   <si>
-    <t xml:space="preserve">7</t>
+    <t>7</t>
   </si>
   <si>
-    <t xml:space="preserve">Extent of Tumor Resection</t>
+    <t>Extent of Tumor Resection</t>
   </si>
   <si>
-    <t xml:space="preserve">8</t>
+    <t>8</t>
   </si>
   <si>
-    <t xml:space="preserve">Cancer predisposition syndrome</t>
+    <t>Age at Chemo Start</t>
   </si>
   <si>
-    <t xml:space="preserve">9</t>
+    <t>9</t>
   </si>
   <si>
-    <t xml:space="preserve">Age at Chemo Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age at Radiation Start</t>
+    <t>Age at Radiation Start</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -139,6 +140,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,14 +430,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,131 +451,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>0.217969285650775</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.606339366063394</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.59454054594540595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.0331966803319668</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>7.1792820717928196E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.228377162283772</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.227077292270773</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.787121287871213</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.78462153784621502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.0612938706129387</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>4.3876295317300799E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="n">
-        <v>0.0438762953173008</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.857686771210749</v>
+      <c r="C10">
+        <v>0.85768677121074899</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,131 +575,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>0.278583212588568</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.405059494050595</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.396660333966603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.262573742625737</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.25547445255474499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.278672132786721</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.28647135286471398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.966403359664034</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.96560343965603401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>0.81790230586425605</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="n">
-        <v>0.817902305864256</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.743616658580255</v>
+      <c r="C10">
+        <v>0.74361665858025505</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -708,120 +699,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.742769798117672</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.74276979811767196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.505149485051495</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.49925007499250101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.0158984101589841</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>1.3898610138986099E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.618238176182382</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.62623737626237397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.12484523805322301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.124845238053223</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.259262165005025</v>
+      <c r="C9">
+        <v>0.25926216500502502</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -832,131 +812,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.332748276516126</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.33274827651612598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.368663133686631</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.37496250374962498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0007999200079992</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>2.9997000299969998E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.498550144985501</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.49725027497250301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.284671532846715</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.27507249275072498</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.171182881711829</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.17238276172382799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.212678732126787</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>0.24820414557905701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="n">
-        <v>0.248204145579057</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.541788422608163</v>
+      <c r="C10">
+        <v>0.54178842260816296</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -967,131 +936,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.967973408969047</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.96797340896904704</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.7996200379962</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.79522047795220496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.837116288371163</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.83091690830916898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.0172982701729827</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>1.7698230176982299E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.668633136686331</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.66943305669433095</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.975602439756024</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>0.415013092936939</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="n">
-        <v>0.415013092936939</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.954992648469679</v>
+      <c r="C10">
+        <v>0.95499264846967902</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1102,120 +1060,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.0928659156743261</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>9.2865915674326102E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.942105789421058</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.94610538946105405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0003999600039996</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>3.9996000399960001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.68953104689531</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.68273172682731698</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.311968803119688</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.314768523147685</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.201379862013799</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.266774530287131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.266774530287131</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.267913906300392</v>
+      <c r="C9">
+        <v>0.26791390630039202</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1226,120 +1173,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.451777445840473</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.45177744584047302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0002999700029997</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>5.9994000599939996E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.149185081491851</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>0.156084391560844</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.0546945305469453</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>5.7094290570942903E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.294770522947705</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.298970102989701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.398860113988601</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.52951924023331998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.52951924023332</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="e">
+      <c r="C9" t="e">
         <v>#N/A</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1350,73 +1286,73 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.0575209855960223</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>5.7520985596022298E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.300569943005699</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.303369663033697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.291870812918708</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>0.28847115288471198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.221877812218778</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.218378162183782</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1427,7 +1363,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1438,32 +1374,21 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1474,84 +1399,84 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.563235079302386</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.56323507930238603</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.905509449055094</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.91210878912108795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0001999800019998</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>1.999800019998E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.250874912508749</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.25037496250375002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.854214578542146</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.85641435856414405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1562,32 +1487,21 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1598,131 +1512,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.314239438737987</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.31423943873798699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.201379862013799</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.18918108189181099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.521047895210479</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.52914708529147103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.784521547845215</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.78882111788821097</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.710928907109289</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.699230076992301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.261273872612739</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>0.79904161443616295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="n">
-        <v>0.799041614436163</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.287436204610943</v>
+      <c r="C10">
+        <v>0.28743620461094299</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1733,131 +1636,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.890643284295059</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.89064328429505901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.783321667833217</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.778522147785221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.477352264773523</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.47905209479052102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.297670232976702</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.293970602939706</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.836516348365164</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.83491650834916498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>0.89609940395460796</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="n">
-        <v>0.896099403954608</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.917400417169167</v>
+      <c r="C10">
+        <v>0.91740041716916698</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1868,120 +1760,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.386472094735832</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.38647209473583199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.913008699130087</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.91130886911308895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.520847915208479</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>0.51264873512648701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.925207479252075</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.92620737926207397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.724727527247275</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.71302869713028705</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.944905509449055</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.31840083313623702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.318400833136237</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.0419697378487613</v>
+      <c r="C9">
+        <v>4.1969737848761297E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1992,120 +1873,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.639586858801544</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.63958685880154398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.126887311268873</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.122687731226877</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0001999800019998</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>3.9996000399960001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.841915808419158</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.84481551844815495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.484551544845515</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.49455054494550499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.166383361663834</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.758448848228512</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.758448848228512</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.588256408874304</v>
+      <c r="C9">
+        <v>0.58825640887430397</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2116,120 +1986,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.938442061412132</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.93844206141213204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.628537146285371</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.626337366263374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0076992300769923</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>9.5990400959903993E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.369163083691631</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.35696430356964298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.277872212778722</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.28187181281871798</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.34418826969203797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.344188269692038</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.272306432618882</v>
+      <c r="C9">
+        <v>0.27230643261888199</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2240,120 +2099,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.983065476660649</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.98306547666064903</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.733826617338266</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>0.73972602739726001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0038996100389961</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>5.7994200579942002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.165083491650835</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.154284571542846</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.58004199580042</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0.58474152584741501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.90539699604932899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.905396996049329</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.993188828441369</v>
+      <c r="C9">
+        <v>0.99318882844136902</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2364,107 +2212,96 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.744389813120937</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>0.74438981312093699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.0970902909709029</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>9.9190080991900798E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.0000999900009999</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>9.9990000999900002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0005999400059994</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>3.9996000399960001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.71002899710029</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0.71152884711528896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>0.71522031900989103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.715220319009891</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="n">
+      <c r="C9">
         <v>0.671059143447022</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update cohort and re-run modules
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -454,7 +454,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.595340465953405</v>
+        <v>0.600739926007399</v>
       </c>
     </row>
     <row r="4">
@@ -487,7 +487,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0688931106889311</v>
+        <v>0.0693930606939306</v>
       </c>
     </row>
     <row r="7">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.224677532246775</v>
+        <v>0.226177382261774</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.773122687731227</v>
+        <v>0.772022797720228</v>
       </c>
     </row>
     <row r="9">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.400659934006599</v>
+        <v>0.398160183981602</v>
       </c>
     </row>
     <row r="4">
@@ -611,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.256974302569743</v>
+        <v>0.261273872612739</v>
       </c>
     </row>
     <row r="7">
@@ -622,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.276772322767723</v>
+        <v>0.278572142785721</v>
       </c>
     </row>
     <row r="8">
@@ -633,7 +633,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.967103289671033</v>
+        <v>0.965103489651035</v>
       </c>
     </row>
     <row r="9">
@@ -702,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.503649635036496</v>
+        <v>0.501649835016498</v>
       </c>
     </row>
     <row r="4">
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0146985301469853</v>
+        <v>0.014998500149985</v>
       </c>
     </row>
     <row r="7">
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.62043795620438</v>
+        <v>0.617738226177382</v>
       </c>
     </row>
     <row r="8">
@@ -815,7 +815,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.372562743725627</v>
+        <v>0.367463253674633</v>
       </c>
     </row>
     <row r="4">
@@ -848,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.496250374962504</v>
+        <v>0.494850514948505</v>
       </c>
     </row>
     <row r="7">
@@ -859,7 +859,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.271572842715728</v>
+        <v>0.276172382761724</v>
       </c>
     </row>
     <row r="8">
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.166283371662834</v>
+        <v>0.173582641735826</v>
       </c>
     </row>
     <row r="9">
@@ -939,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.801019898010199</v>
+        <v>0.800919908009199</v>
       </c>
     </row>
     <row r="4">
@@ -972,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.834416558344166</v>
+        <v>0.84011598840116</v>
       </c>
     </row>
     <row r="7">
@@ -983,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0168983101689831</v>
+        <v>0.0145985401459854</v>
       </c>
     </row>
     <row r="8">
@@ -994,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.664933506649335</v>
+        <v>0.667333266673333</v>
       </c>
     </row>
     <row r="9">
@@ -1063,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.942205779422058</v>
+        <v>0.944305569443056</v>
       </c>
     </row>
     <row r="4">
@@ -1085,7 +1085,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0001999800019998</v>
+        <v>0.0003999600039996</v>
       </c>
     </row>
     <row r="6">
@@ -1096,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.685431456854315</v>
+        <v>0.677232276772323</v>
       </c>
     </row>
     <row r="7">
@@ -1107,7 +1107,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.321067893210679</v>
+        <v>0.30976902309769</v>
       </c>
     </row>
     <row r="8">
@@ -1187,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0003999600039996</v>
+        <v>0.0002999700029997</v>
       </c>
     </row>
     <row r="5">
@@ -1198,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.145885411458854</v>
+        <v>0.149385061493851</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0572942705729427</v>
+        <v>0.0606939306069393</v>
       </c>
     </row>
     <row r="7">
@@ -1220,7 +1220,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.304269573042696</v>
+        <v>0.301569843015698</v>
       </c>
     </row>
     <row r="8">
@@ -1289,7 +1289,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.295070492950705</v>
+        <v>0.163383661633837</v>
       </c>
     </row>
     <row r="4">
@@ -1311,7 +1311,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.284971502849715</v>
+        <v>0.209379062093791</v>
       </c>
     </row>
     <row r="6">
@@ -1333,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.218578142185781</v>
+        <v>0.211578842115788</v>
       </c>
     </row>
     <row r="8">
@@ -1402,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.909309069093091</v>
+        <v>0.912108789121088</v>
       </c>
     </row>
     <row r="4">
@@ -1424,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0001999800019998</v>
       </c>
     </row>
     <row r="6">
@@ -1435,7 +1435,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.25017498250175</v>
+        <v>0.253774622537746</v>
       </c>
     </row>
     <row r="7">
@@ -1446,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.854214578542146</v>
+        <v>0.851214878512149</v>
       </c>
     </row>
     <row r="8">
@@ -1515,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.188781121887811</v>
+        <v>0.188581141885811</v>
       </c>
     </row>
     <row r="4">
@@ -1548,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.53044695530447</v>
+        <v>0.515048495150485</v>
       </c>
     </row>
     <row r="7">
@@ -1559,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.792220777922208</v>
+        <v>0.787321267873213</v>
       </c>
     </row>
     <row r="8">
@@ -1570,7 +1570,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.697530246975302</v>
+        <v>0.693730626937306</v>
       </c>
     </row>
     <row r="9">
@@ -1639,7 +1639,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.780621937806219</v>
+        <v>0.776522347765223</v>
       </c>
     </row>
     <row r="4">
@@ -1672,7 +1672,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.468953104689531</v>
+        <v>0.482451754824518</v>
       </c>
     </row>
     <row r="7">
@@ -1683,7 +1683,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.291770822917708</v>
+        <v>0.296670332966703</v>
       </c>
     </row>
     <row r="8">
@@ -1694,7 +1694,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.845115488451155</v>
+        <v>0.837416258374163</v>
       </c>
     </row>
     <row r="9">
@@ -1752,7 +1752,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.386472094735832</v>
+        <v>0.367226758676688</v>
       </c>
     </row>
     <row r="3">
@@ -1763,7 +1763,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.914208579142086</v>
+        <v>0.802919708029197</v>
       </c>
     </row>
     <row r="4">
@@ -1785,7 +1785,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.526647335266473</v>
+        <v>0.499150084991501</v>
       </c>
     </row>
     <row r="6">
@@ -1796,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.931306869313069</v>
+        <v>0.928107189281072</v>
       </c>
     </row>
     <row r="7">
@@ -1807,7 +1807,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.713228677132287</v>
+        <v>0.84021597840216</v>
       </c>
     </row>
     <row r="8">
@@ -1876,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.123187681231877</v>
+        <v>0.127987201279872</v>
       </c>
     </row>
     <row r="4">
@@ -1898,7 +1898,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0004999500049995</v>
       </c>
     </row>
     <row r="6">
@@ -1909,7 +1909,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0231976802319768</v>
+        <v>0.0233976602339766</v>
       </c>
     </row>
     <row r="7">
@@ -1920,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.843015698430157</v>
+        <v>0.842915708429157</v>
       </c>
     </row>
     <row r="8">
@@ -1931,7 +1931,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.487451254874513</v>
+        <v>0.491050894910509</v>
       </c>
     </row>
     <row r="9">
@@ -2000,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.608239176082392</v>
+        <v>0.614438556144386</v>
       </c>
     </row>
     <row r="4">
@@ -2011,7 +2011,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0000999900009999</v>
+        <v>0.0001999800019998</v>
       </c>
     </row>
     <row r="5">
@@ -2022,7 +2022,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0084991500849915</v>
+        <v>0.0094990500949905</v>
       </c>
     </row>
     <row r="6">
@@ -2033,7 +2033,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.85971402859714</v>
+        <v>0.856814318568143</v>
       </c>
     </row>
     <row r="7">
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.36026397360264</v>
+        <v>0.368763123687631</v>
       </c>
     </row>
     <row r="8">
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.28957104289571</v>
+        <v>0.286371362863714</v>
       </c>
     </row>
     <row r="9">
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.734926507349265</v>
+        <v>0.742225777422258</v>
       </c>
     </row>
     <row r="4">
@@ -2146,7 +2146,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0055994400559944</v>
+        <v>0.0053994600539946</v>
       </c>
     </row>
     <row r="6">
@@ -2157,7 +2157,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.167583241675832</v>
+        <v>0.167883211678832</v>
       </c>
     </row>
     <row r="7">
@@ -2168,7 +2168,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.571742825717428</v>
+        <v>0.582841715828417</v>
       </c>
     </row>
     <row r="8">
@@ -2226,7 +2226,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.744389813120937</v>
+        <v>0.660987736725295</v>
       </c>
     </row>
     <row r="3">
@@ -2237,7 +2237,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0978902109789021</v>
+        <v>0.0426957304269573</v>
       </c>
     </row>
     <row r="4">
@@ -2259,7 +2259,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0011998800119988</v>
       </c>
     </row>
     <row r="6">
@@ -2270,7 +2270,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.719428057194281</v>
+        <v>0.877512248775122</v>
       </c>
     </row>
     <row r="7">
@@ -2281,7 +2281,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.993600639936006</v>
       </c>
     </row>
     <row r="8">
@@ -2292,7 +2292,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="n">
-        <v>0.715220319009891</v>
+        <v>0.555138861058704</v>
       </c>
     </row>
     <row r="9">
@@ -2303,7 +2303,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>0.671059143447022</v>
+        <v>0.655966505077126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun all modules with HGG mis-assignments resolved
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -454,7 +454,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.600739926007399</v>
+        <v>0.605339466053395</v>
       </c>
     </row>
     <row r="4">
@@ -487,7 +487,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0693930606939306</v>
+        <v>0.0717928207179282</v>
       </c>
     </row>
     <row r="7">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.226177382261774</v>
+        <v>0.22017798220178</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.772022797720228</v>
+        <v>0.783321667833217</v>
       </c>
     </row>
     <row r="9">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.398160183981602</v>
+        <v>0.391960803919608</v>
       </c>
     </row>
     <row r="4">
@@ -611,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.261273872612739</v>
+        <v>0.266273372662734</v>
       </c>
     </row>
     <row r="7">
@@ -622,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.278572142785721</v>
+        <v>0.286271372862714</v>
       </c>
     </row>
     <row r="8">
@@ -633,7 +633,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.965103489651035</v>
+        <v>0.965803419658034</v>
       </c>
     </row>
     <row r="9">
@@ -702,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.501649835016498</v>
+        <v>0.492150784921508</v>
       </c>
     </row>
     <row r="4">
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.014998500149985</v>
+        <v>0.0148985101489851</v>
       </c>
     </row>
     <row r="7">
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.617738226177382</v>
+        <v>0.622837716228377</v>
       </c>
     </row>
     <row r="8">
@@ -815,7 +815,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.367463253674633</v>
+        <v>0.377762223777622</v>
       </c>
     </row>
     <row r="4">
@@ -837,7 +837,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0004999500049995</v>
       </c>
     </row>
     <row r="6">
@@ -848,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.494850514948505</v>
+        <v>0.503349665033497</v>
       </c>
     </row>
     <row r="7">
@@ -859,7 +859,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.276172382761724</v>
+        <v>0.277272272772723</v>
       </c>
     </row>
     <row r="8">
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.173582641735826</v>
+        <v>0.171482851714829</v>
       </c>
     </row>
     <row r="9">
@@ -939,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.800919908009199</v>
+        <v>0.797620237976202</v>
       </c>
     </row>
     <row r="4">
@@ -972,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.84011598840116</v>
+        <v>0.831916808319168</v>
       </c>
     </row>
     <row r="7">
@@ -983,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0145985401459854</v>
+        <v>0.0171982801719828</v>
       </c>
     </row>
     <row r="8">
@@ -994,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.667333266673333</v>
+        <v>0.661533846615338</v>
       </c>
     </row>
     <row r="9">
@@ -1063,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.944305569443056</v>
+        <v>0.941805819418058</v>
       </c>
     </row>
     <row r="4">
@@ -1085,7 +1085,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0003999600039996</v>
+        <v>0.0004999500049995</v>
       </c>
     </row>
     <row r="6">
@@ -1096,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.677232276772323</v>
+        <v>0.681231876812319</v>
       </c>
     </row>
     <row r="7">
@@ -1107,7 +1107,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.30976902309769</v>
+        <v>0.314868513148685</v>
       </c>
     </row>
     <row r="8">
@@ -1198,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.149385061493851</v>
+        <v>0.153584641535846</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0606939306069393</v>
+        <v>0.0543945605439456</v>
       </c>
     </row>
     <row r="7">
@@ -1220,7 +1220,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.301569843015698</v>
+        <v>0.299270072992701</v>
       </c>
     </row>
     <row r="8">
@@ -1289,7 +1289,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.163383661633837</v>
+        <v>0.174182581741826</v>
       </c>
     </row>
     <row r="4">
@@ -1311,7 +1311,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.209379062093791</v>
+        <v>0.204479552044796</v>
       </c>
     </row>
     <row r="6">
@@ -1333,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.211578842115788</v>
+        <v>0.211778822117788</v>
       </c>
     </row>
     <row r="8">
@@ -1402,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.912108789121088</v>
+        <v>0.910708929107089</v>
       </c>
     </row>
     <row r="4">
@@ -1424,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0001999800019998</v>
+        <v>0.0000999900009999</v>
       </c>
     </row>
     <row r="6">
@@ -1435,7 +1435,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.253774622537746</v>
+        <v>0.257574242575742</v>
       </c>
     </row>
     <row r="7">
@@ -1446,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.851214878512149</v>
+        <v>0.857514248575142</v>
       </c>
     </row>
     <row r="8">
@@ -1515,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.188581141885811</v>
+        <v>0.2001799820018</v>
       </c>
     </row>
     <row r="4">
@@ -1548,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.515048495150485</v>
+        <v>0.526847315268473</v>
       </c>
     </row>
     <row r="7">
@@ -1559,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.787321267873213</v>
+        <v>0.794020597940206</v>
       </c>
     </row>
     <row r="8">
@@ -1570,7 +1570,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.693730626937306</v>
+        <v>0.695230476952305</v>
       </c>
     </row>
     <row r="9">
@@ -1639,7 +1639,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.776522347765223</v>
+        <v>0.777222277772223</v>
       </c>
     </row>
     <row r="4">
@@ -1672,7 +1672,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.482451754824518</v>
+        <v>0.46965303469653</v>
       </c>
     </row>
     <row r="7">
@@ -1683,7 +1683,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.296670332966703</v>
+        <v>0.293670632936706</v>
       </c>
     </row>
     <row r="8">
@@ -1694,7 +1694,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.837416258374163</v>
+        <v>0.83981601839816</v>
       </c>
     </row>
     <row r="9">
@@ -1763,7 +1763,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.802919708029197</v>
+        <v>0.805019498050195</v>
       </c>
     </row>
     <row r="4">
@@ -1785,7 +1785,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.499150084991501</v>
+        <v>0.505049495050495</v>
       </c>
     </row>
     <row r="6">
@@ -1796,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.928107189281072</v>
+        <v>0.931806819318068</v>
       </c>
     </row>
     <row r="7">
@@ -1807,7 +1807,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.84021597840216</v>
+        <v>0.848115188481152</v>
       </c>
     </row>
     <row r="8">
@@ -1876,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.127987201279872</v>
+        <v>0.127087291270873</v>
       </c>
     </row>
     <row r="4">
@@ -1898,7 +1898,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0004999500049995</v>
+        <v>0.0005999400059994</v>
       </c>
     </row>
     <row r="6">
@@ -1909,7 +1909,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0233976602339766</v>
+        <v>0.0216978302169783</v>
       </c>
     </row>
     <row r="7">
@@ -1920,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.842915708429157</v>
+        <v>0.844015598440156</v>
       </c>
     </row>
     <row r="8">
@@ -1931,7 +1931,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.491050894910509</v>
+        <v>0.48965103489651</v>
       </c>
     </row>
     <row r="9">
@@ -2000,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.614438556144386</v>
+        <v>0.615738426157384</v>
       </c>
     </row>
     <row r="4">
@@ -2011,7 +2011,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0001999800019998</v>
+        <v>0.0000999900009999</v>
       </c>
     </row>
     <row r="5">
@@ -2022,7 +2022,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0094990500949905</v>
+        <v>0.0106989301069893</v>
       </c>
     </row>
     <row r="6">
@@ -2033,7 +2033,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.856814318568143</v>
+        <v>0.856714328567143</v>
       </c>
     </row>
     <row r="7">
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.368763123687631</v>
+        <v>0.359264073592641</v>
       </c>
     </row>
     <row r="8">
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.286371362863714</v>
+        <v>0.275672432756724</v>
       </c>
     </row>
     <row r="9">
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.742225777422258</v>
+        <v>0.738426157384262</v>
       </c>
     </row>
     <row r="4">
@@ -2146,7 +2146,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0053994600539946</v>
+        <v>0.0063993600639936</v>
       </c>
     </row>
     <row r="6">
@@ -2157,7 +2157,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.167883211678832</v>
+        <v>0.163283671632837</v>
       </c>
     </row>
     <row r="7">
@@ -2168,7 +2168,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.582841715828417</v>
+        <v>0.573942605739426</v>
       </c>
     </row>
     <row r="8">
@@ -2237,7 +2237,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0426957304269573</v>
+        <v>0.0477952204779522</v>
       </c>
     </row>
     <row r="4">
@@ -2259,7 +2259,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0011998800119988</v>
+        <v>0.0005999400059994</v>
       </c>
     </row>
     <row r="6">
@@ -2270,7 +2270,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.877512248775122</v>
+        <v>0.877212278772123</v>
       </c>
     </row>
     <row r="7">
@@ -2281,7 +2281,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.993600639936006</v>
+        <v>0.991300869913009</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
plot HGG/DMG mol subtype dist by superpop
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -454,7 +454,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.601339866013399</v>
+        <v>0.606439356064394</v>
       </c>
     </row>
     <row r="4">
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.218578142185781</v>
+        <v>0.22027797220278</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.776022397760224</v>
+        <v>0.78002199780022</v>
       </c>
     </row>
     <row r="9">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.398060193980602</v>
+        <v>0.395560443955604</v>
       </c>
     </row>
     <row r="4">
@@ -611,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.253774622537746</v>
+        <v>0.263373662633737</v>
       </c>
     </row>
     <row r="7">
@@ -622,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.285471452854715</v>
+        <v>0.279372062793721</v>
       </c>
     </row>
     <row r="8">
@@ -633,7 +633,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.968303169683032</v>
+        <v>0.966803319668033</v>
       </c>
     </row>
     <row r="9">
@@ -691,7 +691,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.742769798117672</v>
+        <v>0.652232662013525</v>
       </c>
     </row>
     <row r="3">
@@ -702,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5003499650035</v>
+        <v>0.618438156184382</v>
       </c>
     </row>
     <row r="4">
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0138986101389861</v>
+        <v>0.017998200179982</v>
       </c>
     </row>
     <row r="7">
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.625137486251375</v>
+        <v>0.777622237776222</v>
       </c>
     </row>
     <row r="8">
@@ -815,7 +815,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.372262773722628</v>
+        <v>0.367763223677632</v>
       </c>
     </row>
     <row r="4">
@@ -837,7 +837,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0002999700029997</v>
+        <v>0.0003999600039996</v>
       </c>
     </row>
     <row r="6">
@@ -848,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.491450854914509</v>
+        <v>0.514048595140486</v>
       </c>
     </row>
     <row r="7">
@@ -859,7 +859,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.273272672732727</v>
+        <v>0.273872612738726</v>
       </c>
     </row>
     <row r="8">
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.171082891710829</v>
+        <v>0.17048295170483</v>
       </c>
     </row>
     <row r="9">
@@ -928,7 +928,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.967973408969047</v>
+        <v>0.957322984148866</v>
       </c>
     </row>
     <row r="3">
@@ -939,7 +939,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.789221077892211</v>
+        <v>0.568943105689431</v>
       </c>
     </row>
     <row r="4">
@@ -972,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.841515848415158</v>
+        <v>0.803219678032197</v>
       </c>
     </row>
     <row r="7">
@@ -983,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0161983801619838</v>
+        <v>0.012998700129987</v>
       </c>
     </row>
     <row r="8">
@@ -994,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.657334266573343</v>
+        <v>0.661933806619338</v>
       </c>
     </row>
     <row r="9">
@@ -1063,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.939406059394061</v>
+        <v>0.93950604939506</v>
       </c>
     </row>
     <row r="4">
@@ -1085,7 +1085,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0004999500049995</v>
+        <v>0.0007999200079992</v>
       </c>
     </row>
     <row r="6">
@@ -1096,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.683831616838316</v>
+        <v>0.683131686831317</v>
       </c>
     </row>
     <row r="7">
@@ -1107,7 +1107,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.316368363163684</v>
+        <v>0.318868113188681</v>
       </c>
     </row>
     <row r="8">
@@ -1187,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0004999500049995</v>
+        <v>0.0003999600039996</v>
       </c>
     </row>
     <row r="5">
@@ -1198,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.147385261473853</v>
+        <v>0.145385461453855</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0578942105789421</v>
+        <v>0.0598940105989401</v>
       </c>
     </row>
     <row r="7">
@@ -1220,7 +1220,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.306469353064694</v>
+        <v>0.304569543045695</v>
       </c>
     </row>
     <row r="8">
@@ -1289,7 +1289,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.17048295170483</v>
+        <v>0.168683131686831</v>
       </c>
     </row>
     <row r="4">
@@ -1311,7 +1311,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.207979202079792</v>
+        <v>0.21037896210379</v>
       </c>
     </row>
     <row r="6">
@@ -1333,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.210578942105789</v>
+        <v>0.215478452154785</v>
       </c>
     </row>
     <row r="8">
@@ -1402,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.914908509149085</v>
+        <v>0.917908209179082</v>
       </c>
     </row>
     <row r="4">
@@ -1435,7 +1435,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.256974302569743</v>
+        <v>0.26037396260374</v>
       </c>
     </row>
     <row r="7">
@@ -1446,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.854614538546145</v>
+        <v>0.863813618638136</v>
       </c>
     </row>
     <row r="8">
@@ -1515,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.189181081891811</v>
+        <v>0.2004799520048</v>
       </c>
     </row>
     <row r="4">
@@ -1548,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.521747825217478</v>
+        <v>0.538446155384462</v>
       </c>
     </row>
     <row r="7">
@@ -1559,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.789321067893211</v>
+        <v>0.789221077892211</v>
       </c>
     </row>
     <row r="8">
@@ -1570,7 +1570,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.696030396960304</v>
+        <v>0.695630436956304</v>
       </c>
     </row>
     <row r="9">
@@ -1639,7 +1639,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.781821817818218</v>
+        <v>0.780621937806219</v>
       </c>
     </row>
     <row r="4">
@@ -1672,7 +1672,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.46985301469853</v>
+        <v>0.475852414758524</v>
       </c>
     </row>
     <row r="7">
@@ -1683,7 +1683,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.297170282971703</v>
+        <v>0.304069593040696</v>
       </c>
     </row>
     <row r="8">
@@ -1694,7 +1694,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.83011698830117</v>
+        <v>0.833216678332167</v>
       </c>
     </row>
     <row r="9">
@@ -1763,7 +1763,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8000199980002</v>
+        <v>0.806119388061194</v>
       </c>
     </row>
     <row r="4">
@@ -1785,7 +1785,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.501449855014499</v>
+        <v>0.502549745025497</v>
       </c>
     </row>
     <row r="6">
@@ -1796,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.932206779322068</v>
+        <v>0.934406559344066</v>
       </c>
     </row>
     <row r="7">
@@ -1807,7 +1807,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.848215178482152</v>
+        <v>0.847915208479152</v>
       </c>
     </row>
     <row r="8">
@@ -1876,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.123687631236876</v>
+        <v>0.126187381261874</v>
       </c>
     </row>
     <row r="4">
@@ -1909,7 +1909,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0195980401959804</v>
+        <v>0.0217978202179782</v>
       </c>
     </row>
     <row r="7">
@@ -1920,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.846915308469153</v>
+        <v>0.848115188481152</v>
       </c>
     </row>
     <row r="8">
@@ -1931,7 +1931,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.484651534846515</v>
+        <v>0.485651434856514</v>
       </c>
     </row>
     <row r="9">
@@ -2000,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.615938406159384</v>
+        <v>0.623437656234377</v>
       </c>
     </row>
     <row r="4">
@@ -2022,7 +2022,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0102989701029897</v>
+        <v>0.0085991400859914</v>
       </c>
     </row>
     <row r="6">
@@ -2033,7 +2033,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.854114588541146</v>
+        <v>0.852514748525148</v>
       </c>
     </row>
     <row r="7">
@@ -2044,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.358864113588641</v>
+        <v>0.365863413658634</v>
       </c>
     </row>
     <row r="8">
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.278472152784722</v>
+        <v>0.269273072692731</v>
       </c>
     </row>
     <row r="9">
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.741025897410259</v>
+        <v>0.740925907409259</v>
       </c>
     </row>
     <row r="4">
@@ -2146,7 +2146,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0050994900509949</v>
+        <v>0.004999500049995</v>
       </c>
     </row>
     <row r="6">
@@ -2157,7 +2157,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.166083391660834</v>
+        <v>0.16988301169883</v>
       </c>
     </row>
     <row r="7">
@@ -2168,7 +2168,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.598840115988401</v>
+        <v>0.570642935706429</v>
       </c>
     </row>
     <row r="8">
@@ -2237,7 +2237,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0417958204179582</v>
+        <v>0.0491950804919508</v>
       </c>
     </row>
     <row r="4">
@@ -2259,7 +2259,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0006999300069993</v>
+        <v>0.0003999600039996</v>
       </c>
     </row>
     <row r="6">
@@ -2270,7 +2270,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.874712528747125</v>
+        <v>0.87971202879712</v>
       </c>
     </row>
     <row r="7">
@@ -2281,7 +2281,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.993600639936006</v>
+        <v>0.992800719928007</v>
       </c>
     </row>
     <row r="8">

</xml_diff>